<commit_message>
auswertung fast fertig - nur temperaturkurve fehlt noch
</commit_message>
<xml_diff>
--- a/K225/auswertung/fits.xlsx
+++ b/K225/auswertung/fits.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>n</t>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>lnsct</t>
+  </si>
+  <si>
+    <t>dtauf</t>
+  </si>
+  <si>
+    <t>dsct</t>
+  </si>
+  <si>
+    <t>d1/T</t>
+  </si>
+  <si>
+    <t>dlnsct</t>
   </si>
 </sst>
 </file>
@@ -358,11 +370,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="233560704"/>
-        <c:axId val="233841024"/>
+        <c:axId val="211094528"/>
+        <c:axId val="211108608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="233560704"/>
+        <c:axId val="211094528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -372,12 +384,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233841024"/>
+        <c:crossAx val="211108608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="233841024"/>
+        <c:axId val="211108608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -388,7 +400,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233560704"/>
+        <c:crossAx val="211094528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -624,11 +636,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="233878272"/>
-        <c:axId val="233879808"/>
+        <c:axId val="211145856"/>
+        <c:axId val="211147392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="233878272"/>
+        <c:axId val="211145856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -638,12 +650,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233879808"/>
+        <c:crossAx val="211147392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="233879808"/>
+        <c:axId val="211147392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -654,7 +666,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233878272"/>
+        <c:crossAx val="211145856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -705,7 +717,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle4!$Y$4</c:f>
+              <c:f>Tabelle4!$AB$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -721,7 +733,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle4!$X$5:$X$13</c:f>
+              <c:f>Tabelle4!$Z$5:$Z$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -757,7 +769,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle4!$Y$5:$Y$13</c:f>
+              <c:f>Tabelle4!$AB$5:$AB$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -801,11 +813,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="241439104"/>
-        <c:axId val="241428736"/>
+        <c:axId val="211433728"/>
+        <c:axId val="211435520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="241439104"/>
+        <c:axId val="211433728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -815,12 +827,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="241428736"/>
+        <c:crossAx val="211435520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="241428736"/>
+        <c:axId val="211435520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -831,7 +843,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="241439104"/>
+        <c:crossAx val="211433728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -868,7 +880,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -998,11 +1009,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="175140224"/>
-        <c:axId val="175138688"/>
+        <c:axId val="209056896"/>
+        <c:axId val="209058432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="175140224"/>
+        <c:axId val="209056896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1012,12 +1023,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175138688"/>
+        <c:crossAx val="209058432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="175138688"/>
+        <c:axId val="209058432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1028,14 +1039,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175140224"/>
+        <c:crossAx val="209056896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1120,7 +1130,7 @@
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>585787</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -1467,15 +1477,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:Y13"/>
+  <dimension ref="C4:AC13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M19" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4:Y13"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -1537,16 +1547,28 @@
         <v>19</v>
       </c>
       <c r="W4" t="s">
+        <v>26</v>
+      </c>
+      <c r="X4" t="s">
         <v>23</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z4" t="s">
         <v>24</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AA4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB4" t="s">
         <v>25</v>
       </c>
+      <c r="AC4" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="5" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>1</v>
       </c>
@@ -1617,19 +1639,35 @@
         <v>55.139480941582804</v>
       </c>
       <c r="W5">
+        <f>V5^2*SQRT((Q5/H5)^2+(P5*I5/H5^2)^2+(S5/F5)^2+(R5*G5/F5^2)^2)</f>
+        <v>27.674029578434759</v>
+      </c>
+      <c r="X5">
         <f>(T5-V5)/V5/(F5-T5)</f>
         <v>4.6679955901698716E-3</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
+        <f>X5*SQRT((U5^2+W5^2)/(T5-V5)^2+(W5/V5)^2+(G5^2+T5^2)/(F5-T5)^2)</f>
+        <v>2.5793318320408053E-2</v>
+      </c>
+      <c r="Z5">
         <f>1/(D5+273.15)</f>
         <v>3.331667499583542E-3</v>
       </c>
-      <c r="Y5">
-        <f>LOG(W5)</f>
+      <c r="AA5">
+        <f>E5*Z5^2</f>
+        <v>1.1100008327781251E-5</v>
+      </c>
+      <c r="AB5">
+        <f>LOG(X5)</f>
         <v>-2.3308695629021163</v>
       </c>
+      <c r="AC5">
+        <f>-Y5/AB5</f>
+        <v>1.1065963849256901E-2</v>
+      </c>
     </row>
-    <row r="6" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>2</v>
       </c>
@@ -1700,19 +1738,35 @@
         <v>45.243178274129534</v>
       </c>
       <c r="W6">
-        <f t="shared" ref="W6:W13" si="9">(T6-V6)/V6/(F6-T6)</f>
+        <f t="shared" ref="W6:W13" si="9">V6^2*SQRT((Q6/H6)^2+(P6*I6/H6^2)^2+(S6/F6)^2+(R6*G6/F6^2)^2)</f>
+        <v>6.4301677292027346</v>
+      </c>
+      <c r="X6">
+        <f t="shared" ref="X6:X13" si="10">(T6-V6)/V6/(F6-T6)</f>
         <v>1.700937445318574E-2</v>
       </c>
-      <c r="X6">
-        <f t="shared" ref="X6:X13" si="10">1/(D6+273.15)</f>
+      <c r="Y6">
+        <f t="shared" ref="Y6:Y13" si="11">X6*SQRT((U6^2+W6^2)/(T6-V6)^2+(W6/V6)^2+(G6^2+T6^2)/(F6-T6)^2)</f>
+        <v>4.9022773963592475E-2</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" ref="Z6:Z13" si="12">1/(D6+273.15)</f>
         <v>3.0473868657626088E-3</v>
       </c>
-      <c r="Y6">
-        <f t="shared" ref="Y6:Y13" si="11">LOG(W6)</f>
+      <c r="AA6">
+        <f t="shared" ref="AA6:AA13" si="13">E6*Z6^2</f>
+        <v>9.2865667096224553E-6</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" ref="AB6:AB13" si="14">LOG(X6)</f>
         <v>-1.7693116579644517</v>
       </c>
+      <c r="AC6">
+        <f t="shared" ref="AC6:AC13" si="15">-Y6/AB6</f>
+        <v>2.7707257646169547E-2</v>
+      </c>
     </row>
-    <row r="7" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>3</v>
       </c>
@@ -1784,18 +1838,34 @@
       </c>
       <c r="W7">
         <f t="shared" si="9"/>
-        <v>2.6058448742370663E-2</v>
+        <v>8.1252938393354466</v>
       </c>
       <c r="X7">
         <f t="shared" si="10"/>
-        <v>2.9926679634894511E-3</v>
+        <v>2.6058448742370663E-2</v>
       </c>
       <c r="Y7">
         <f t="shared" si="11"/>
+        <v>0.10936463305413245</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="12"/>
+        <v>2.9926679634894511E-3</v>
+      </c>
+      <c r="AA7">
+        <f t="shared" si="13"/>
+        <v>8.9560615396960976E-6</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" si="14"/>
         <v>-1.5840514413740392</v>
       </c>
+      <c r="AC7">
+        <f t="shared" si="15"/>
+        <v>6.9041086796567216E-2</v>
+      </c>
     </row>
-    <row r="8" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>4</v>
       </c>
@@ -1867,18 +1937,34 @@
       </c>
       <c r="W8">
         <f t="shared" si="9"/>
-        <v>1.0535505543021208E-2</v>
+        <v>14.800163020329787</v>
       </c>
       <c r="X8">
         <f t="shared" si="10"/>
-        <v>2.9312619082515023E-3</v>
+        <v>1.0535505543021208E-2</v>
       </c>
       <c r="Y8">
         <f t="shared" si="11"/>
+        <v>3.7463073546343116E-2</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="12"/>
+        <v>2.9312619082515023E-3</v>
+      </c>
+      <c r="AA8">
+        <f t="shared" si="13"/>
+        <v>8.5922963747662392E-6</v>
+      </c>
+      <c r="AB8">
+        <f t="shared" si="14"/>
         <v>-1.9773446200675788</v>
       </c>
+      <c r="AC8">
+        <f t="shared" si="15"/>
+        <v>1.8946152919496025E-2</v>
+      </c>
     </row>
-    <row r="9" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>5</v>
       </c>
@@ -1950,18 +2036,34 @@
       </c>
       <c r="W9">
         <f t="shared" si="9"/>
-        <v>2.2538098953661368E-2</v>
+        <v>7.1833613646223453</v>
       </c>
       <c r="X9">
         <f t="shared" si="10"/>
-        <v>2.847785846504343E-3</v>
+        <v>2.2538098953661368E-2</v>
       </c>
       <c r="Y9">
         <f t="shared" si="11"/>
+        <v>8.0782195496747422E-2</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="12"/>
+        <v>2.847785846504343E-3</v>
+      </c>
+      <c r="AA9">
+        <f t="shared" si="13"/>
+        <v>8.1098842275504576E-6</v>
+      </c>
+      <c r="AB9">
+        <f t="shared" si="14"/>
         <v>-1.6470827186693811</v>
       </c>
+      <c r="AC9">
+        <f t="shared" si="15"/>
+        <v>4.9045621437888959E-2</v>
+      </c>
     </row>
-    <row r="10" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>6</v>
       </c>
@@ -2033,18 +2135,34 @@
       </c>
       <c r="W10">
         <f t="shared" si="9"/>
-        <v>5.6290358691710373E-3</v>
+        <v>17.721144851227379</v>
       </c>
       <c r="X10">
         <f t="shared" si="10"/>
-        <v>2.8236622899901172E-3</v>
+        <v>5.6290358691710373E-3</v>
       </c>
       <c r="Y10">
         <f t="shared" si="11"/>
+        <v>1.9990537785302773E-2</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="12"/>
+        <v>2.8236622899901172E-3</v>
+      </c>
+      <c r="AA10">
+        <f t="shared" si="13"/>
+        <v>7.973068727912233E-6</v>
+      </c>
+      <c r="AB10">
+        <f t="shared" si="14"/>
         <v>-2.2495659839329014</v>
       </c>
+      <c r="AC10">
+        <f t="shared" si="15"/>
+        <v>8.8863976109531343E-3</v>
+      </c>
     </row>
-    <row r="11" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>7</v>
       </c>
@@ -2116,18 +2234,34 @@
       </c>
       <c r="W11">
         <f t="shared" si="9"/>
-        <v>8.1339181385428009E-3</v>
+        <v>20.589869928601079</v>
       </c>
       <c r="X11">
         <f t="shared" si="10"/>
-        <v>2.7162841233192994E-3</v>
+        <v>8.1339181385428009E-3</v>
       </c>
       <c r="Y11">
         <f t="shared" si="11"/>
+        <v>3.7437772926802143E-2</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="12"/>
+        <v>2.7162841233192994E-3</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" si="13"/>
+        <v>7.3781994385964948E-6</v>
+      </c>
+      <c r="AB11">
+        <f t="shared" si="14"/>
         <v>-2.0897002027401408</v>
       </c>
+      <c r="AC11">
+        <f t="shared" si="15"/>
+        <v>1.7915379860571137E-2</v>
+      </c>
     </row>
-    <row r="12" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>8</v>
       </c>
@@ -2199,18 +2333,34 @@
       </c>
       <c r="W12">
         <f t="shared" si="9"/>
-        <v>1.6485536195819859E-2</v>
+        <v>8.7063166979067432</v>
       </c>
       <c r="X12">
         <f t="shared" si="10"/>
-        <v>2.6236389872753511E-3</v>
+        <v>1.6485536195819859E-2</v>
       </c>
       <c r="Y12">
         <f t="shared" si="11"/>
+        <v>6.6263611684374696E-2</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="12"/>
+        <v>2.6236389872753511E-3</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="13"/>
+        <v>6.8834815355512294E-6</v>
+      </c>
+      <c r="AB12">
+        <f t="shared" si="14"/>
         <v>-1.7828969227641573</v>
       </c>
+      <c r="AC12">
+        <f t="shared" si="15"/>
+        <v>3.7166260616817548E-2</v>
+      </c>
     </row>
-    <row r="13" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>9</v>
       </c>
@@ -2282,15 +2432,31 @@
       </c>
       <c r="W13">
         <f t="shared" si="9"/>
-        <v>2.2890125045270618E-2</v>
+        <v>9.8407331710664199</v>
       </c>
       <c r="X13">
         <f t="shared" si="10"/>
-        <v>2.5371051630090069E-3</v>
+        <v>2.2890125045270618E-2</v>
       </c>
       <c r="Y13">
         <f t="shared" si="11"/>
+        <v>0.11203656454766082</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="12"/>
+        <v>2.5371051630090069E-3</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" si="13"/>
+        <v>6.4369026081669598E-6</v>
+      </c>
+      <c r="AB13">
+        <f t="shared" si="14"/>
         <v>-1.6403518348342958</v>
+      </c>
+      <c r="AC13">
+        <f t="shared" si="15"/>
+        <v>6.8300325679203133E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>